<commit_message>
#355 ExcelSchemaBuilder uses 2 header lines and merged cell format
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderAttribute.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderAttribute.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A2CE9-51F1-45B0-8CAF-CCB6C9AACB51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BEACC5-D9E3-4F24-887E-033788874007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="2070" windowWidth="20370" windowHeight="11430" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>WrongMultiplicity</t>
+  </si>
+  <si>
+    <t>xsd</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -742,6 +745,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1098,121 +1107,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB625F5E-6BDB-4C05-BB93-12E3BD870C50}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.53515625" customWidth="1"/>
-    <col min="2" max="2" width="16.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" customWidth="1"/>
-    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" customWidth="1"/>
-    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1220,54 +1239,64 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287548FE-BF2B-47D2-9F17-07261DB3E72B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="17.69140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1275,66 +1304,78 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD8192E-49C0-4792-991A-D63BBCDA3251}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="3" width="17.3828125" customWidth="1"/>
-    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" customWidth="1"/>
-    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1342,55 +1383,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1051FC8A-45FF-430E-806F-18C2C91AFA50}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="13.3046875" customWidth="1"/>
-    <col min="4" max="4" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.3828125" customWidth="1"/>
-    <col min="7" max="7" width="17.69140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1398,62 +1449,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C65980-0B1B-4CAD-8672-FF8AE8F17C37}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="12.15234375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1461,51 +1522,61 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F233A195-0548-499C-A6F3-48420E331EF4}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="12.15234375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1513,99 +1584,110 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CA0F3F-D6D3-4156-AD15-7844900A3854}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="3" width="17.3828125" customWidth="1"/>
-    <col min="4" max="4" width="12.15234375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1613,94 +1695,88 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E541D522-2E1B-4544-8069-54D92B113960}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.23046875" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.3828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="F4">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="E4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1708,22 +1784,42 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1731,54 +1827,64 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BC5114-E86A-4509-9711-F7E3B127020F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.61328125" customWidth="1"/>
-    <col min="2" max="2" width="12.15234375" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="17.69140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1786,54 +1892,64 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A9775B-918C-4A83-A4AE-FA22E877E548}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="23.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="17.69140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1841,54 +1957,64 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35032079-5C26-4C12-99C9-D449945A5E02}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="17.3828125" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.3828125" customWidth="1"/>
-    <col min="6" max="6" width="17.69140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>